<commit_message>
Switched from Obj to Thing for final prize to preemptively prevent some issues with Objs id collisions.
</commit_message>
<xml_diff>
--- a/resources/LangMod/CN/KiriaSources.xlsx
+++ b/resources/LangMod/CN/KiriaSources.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Chara" sheetId="1" state="visible" r:id="rId3"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="243">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -833,7 +833,8 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">的地图，找出那里有什么。\n（尝试在世界地图上挖掘。）</t>
+      <t xml:space="preserve">的地图，找出那里有什么。
+（尝试在世界地图上挖掘。）</t>
     </r>
     <r>
       <rPr>
@@ -1122,6 +1123,18 @@
   </si>
   <si>
     <t xml:space="preserve">它具有类似生物的基因特征。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">corpse_ryozu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ext</t>
+  </si>
+  <si>
+    <t xml:space="preserve">653,652,656,657,658,659,-659</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KiriaCorpse</t>
   </si>
   <si>
     <t xml:space="preserve">parent</t>
@@ -1233,7 +1246,7 @@
     <numFmt numFmtId="166" formatCode="#,##0"/>
     <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1347,6 +1360,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1390,7 +1410,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1488,6 +1508,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1693,7 +1717,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
+      <selection pane="bottomLeft" activeCell="G26" activeCellId="1" sqref="F7 G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2404,7 +2428,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+      <selection pane="bottomLeft" activeCell="H10" activeCellId="1" sqref="F7 H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2588,7 +2612,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N22" activeCellId="0" sqref="N22"/>
+      <selection pane="topLeft" activeCell="N22" activeCellId="1" sqref="F7 N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2613,7 +2637,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="D4" activeCellId="1" sqref="F7 D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2966,10 +2990,10 @@
   </sheetPr>
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="M16" activeCellId="0" sqref="M16"/>
+      <selection pane="bottomLeft" activeCell="M17" activeCellId="1" sqref="F7 M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3032,7 +3056,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
         <v>140</v>
       </c>
@@ -3060,7 +3084,7 @@
       <c r="L4" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="10" t="s">
         <v>146</v>
       </c>
       <c r="N4" s="6" t="n">
@@ -3083,12 +3107,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BT6"/>
+  <dimension ref="A1:BT7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AR1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="AR1" activeCellId="0" sqref="AR1"/>
-      <selection pane="bottomLeft" activeCell="AZ6" activeCellId="0" sqref="AZ6"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3814,6 +3838,102 @@
         <v>205</v>
       </c>
     </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="0"/>
+      <c r="D7" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="E7" s="0"/>
+      <c r="F7" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="G7" s="0"/>
+      <c r="H7" s="0"/>
+      <c r="I7" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="J7" s="0"/>
+      <c r="K7" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="L7" s="0"/>
+      <c r="M7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="O7" s="0"/>
+      <c r="P7" s="0"/>
+      <c r="Q7" s="0"/>
+      <c r="R7" s="0"/>
+      <c r="S7" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="T7" s="0"/>
+      <c r="U7" s="0"/>
+      <c r="V7" s="0"/>
+      <c r="W7" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="X7" s="0"/>
+      <c r="Y7" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z7" s="0"/>
+      <c r="AA7" s="1" t="n">
+        <v>2686</v>
+      </c>
+      <c r="AB7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AF7" s="1" t="n">
+        <v>4000</v>
+      </c>
+      <c r="AG7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="AI7" s="0"/>
+      <c r="AJ7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK7" s="0"/>
+      <c r="AL7" s="0"/>
+      <c r="AM7" s="0"/>
+      <c r="AN7" s="0"/>
+      <c r="AO7" s="0"/>
+      <c r="AP7" s="0"/>
+      <c r="AQ7" s="0"/>
+      <c r="AR7" s="0"/>
+      <c r="AS7" s="0"/>
+      <c r="AT7" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AU7" s="0"/>
+      <c r="AV7" s="0"/>
+      <c r="AW7" s="0"/>
+      <c r="AX7" s="0"/>
+      <c r="AY7" s="0"/>
+      <c r="AZ7" s="0"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3835,7 +3955,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="H8" activeCellId="1" sqref="F7 H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3867,215 +3987,215 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>206</v>
-      </c>
-      <c r="C1" s="25" t="s">
+      <c r="A1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="25" t="s">
-        <v>207</v>
-      </c>
-      <c r="I1" s="25" t="s">
+      <c r="H1" s="26" t="s">
+        <v>211</v>
+      </c>
+      <c r="I1" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="J1" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="K1" s="25" t="s">
-        <v>209</v>
-      </c>
-      <c r="L1" s="25" t="s">
-        <v>210</v>
-      </c>
-      <c r="M1" s="25" t="s">
-        <v>211</v>
-      </c>
-      <c r="N1" s="25" t="s">
+      <c r="J1" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="O1" s="25" t="s">
+      <c r="K1" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="O1" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="25" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q1" s="25" t="s">
-        <v>214</v>
-      </c>
-      <c r="R1" s="25" t="s">
-        <v>215</v>
-      </c>
-      <c r="S1" s="25" t="s">
-        <v>216</v>
-      </c>
-      <c r="T1" s="25" t="s">
+      <c r="P1" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="U1" s="25" t="s">
+      <c r="Q1" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="V1" s="25" t="s">
+      <c r="R1" s="26" t="s">
         <v>219</v>
       </c>
-      <c r="W1" s="25" t="s">
+      <c r="S1" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="T1" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="U1" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="V1" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="W1" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="X1" s="25" t="s">
+      <c r="X1" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="Y1" s="26"/>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="25" t="s">
+      <c r="A2" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="25" t="s">
+      <c r="H2" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="25" t="s">
+      <c r="J2" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="L2" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="N2" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="O2" s="25" t="s">
+      <c r="L2" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="P2" s="25" t="s">
+      <c r="P2" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="Q2" s="25" t="s">
+      <c r="Q2" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="R2" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="S2" s="25" t="s">
+      <c r="R2" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="S2" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="T2" s="25" t="s">
+      <c r="T2" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="U2" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="V2" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="W2" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="X2" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y2" s="26"/>
-      <c r="Z2" s="26"/>
-      <c r="AA2" s="26"/>
+      <c r="U2" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="V2" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="W2" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="X2" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="25" t="s">
-        <v>220</v>
-      </c>
-      <c r="F3" s="25" t="n">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="F3" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="G3" s="25" t="n">
+      <c r="G3" s="26" t="n">
         <v>100</v>
       </c>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="25" t="s">
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="S3" s="26"/>
-      <c r="T3" s="26"/>
-      <c r="U3" s="26"/>
-      <c r="V3" s="26"/>
-      <c r="W3" s="26"/>
-      <c r="X3" s="26"/>
-      <c r="Y3" s="26"/>
-      <c r="Z3" s="26"/>
-      <c r="AA3" s="26"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="U3" s="27"/>
+      <c r="V3" s="27"/>
+      <c r="W3" s="27"/>
+      <c r="X3" s="27"/>
+      <c r="Y3" s="27"/>
+      <c r="Z3" s="27"/>
+      <c r="AA3" s="27"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="F4" s="6" t="n">
         <v>27</v>
@@ -4087,16 +4207,16 @@
         <v>0</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="P4" s="6" t="n">
         <v>0</v>
@@ -4105,30 +4225,30 @@
         <v>0</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="U4" s="7" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="V4" s="24" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="F5" s="6" t="n">
         <v>1</v>
@@ -4140,7 +4260,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="L5" s="6" t="s">
         <v>63</v>
@@ -4152,13 +4272,13 @@
         <v>0</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="V5" s="24" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Forgot to add the map replace quests to the chinese version of the sources.
</commit_message>
<xml_diff>
--- a/resources/LangMod/CN/KiriaSources.xlsx
+++ b/resources/LangMod/CN/KiriaSources.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Chara" sheetId="1" state="visible" r:id="rId3"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="250">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -389,11 +389,11 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
-        <charset val="134"/>
+        <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">人形控仍然需要一些惩罚...</t>
+      <t xml:space="preserve">人形控仍然需要一些惩罚</t>
     </r>
     <r>
       <rPr>
@@ -403,16 +403,16 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">"
+      <t xml:space="preserve">..."
 "</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
-        <charset val="134"/>
+        <charset val="128"/>
       </rPr>
       <t xml:space="preserve">毕竟我也不是破铜烂铁。</t>
     </r>
@@ -834,118 +834,29 @@
         <charset val="128"/>
       </rPr>
       <t xml:space="preserve">的地图，找出那里有什么。
-（尝试在世界地图上挖掘。）</t>
+（尝试在世界地图上挖掘。）|一支机利亚军队？！保卫自己...|你活下来了，也许楼梯会解锁？|你找到了一个奇怪的实验室，寻找线索。|残骸紧握着一个里面有东西的胶囊？</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">|</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">一支</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">机利亚</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">军队？！保卫自己</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">...|</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">你活下来了，也许楼梯会解锁？</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">|</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">你找到了一个奇怪的实验室，寻找线索。</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">|</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">残骸</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">紧握着一个里面有东西的胶囊？</t>
-    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">kiria_map_replace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lost map?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mod_KiriaDLC.QuestMapReplace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kiriaDLC,mapReplace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">地図をなくしちゃったの？新しいのを描きますよ。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">你地图丢了吗？我可以画一张新的。</t>
   </si>
   <si>
     <t xml:space="preserve">unknown_JP</t>
@@ -1240,11 +1151,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="#,##0"/>
-    <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
   <fonts count="17">
     <font>
@@ -1410,7 +1320,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1471,7 +1381,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1495,6 +1405,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1508,10 +1426,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1717,7 +1631,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G26" activeCellId="1" sqref="F7 G26"/>
+      <selection pane="bottomLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2428,7 +2342,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="H10" activeCellId="1" sqref="F7 H10"/>
+      <selection pane="bottomLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2576,7 +2490,7 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="36.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
         <v>95</v>
       </c>
@@ -2612,7 +2526,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N22" activeCellId="1" sqref="F7 N22"/>
+      <selection pane="topLeft" activeCell="N22" activeCellId="0" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2632,12 +2546,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AG4"/>
+  <dimension ref="A1:AG5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D4" activeCellId="1" sqref="F7 D4"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2871,7 +2785,7 @@
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="15" t="n">
         <f aca="false">MAX(A4:A10058)</f>
-        <v>118</v>
+        <v>1119</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="16" t="s">
@@ -2934,7 +2848,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="n">
-        <v>118</v>
+        <v>1119</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>124</v>
@@ -2972,6 +2886,7 @@
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
     </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2988,17 +2903,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="M17" activeCellId="1" sqref="F7 M17"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="24.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="215.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="208"/>
   </cols>
@@ -3056,7 +2972,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
         <v>140</v>
       </c>
@@ -3090,6 +3006,42 @@
       <c r="N4" s="6" t="n">
         <v>0</v>
       </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="M5" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3109,7 +3061,7 @@
   </sheetPr>
   <dimension ref="A1:BT7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
@@ -3179,22 +3131,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>32</v>
@@ -3215,13 +3167,13 @@
         <v>10</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>8</v>
@@ -3242,15 +3194,15 @@
         <v>13</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="Y1" s="3" t="s">
         <v>14</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="AA1" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="AA1" s="23" t="s">
         <v>111</v>
       </c>
       <c r="AB1" s="3" t="s">
@@ -3263,13 +3215,13 @@
         <v>17</v>
       </c>
       <c r="AE1" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="AF1" s="21" t="s">
-        <v>158</v>
+        <v>164</v>
+      </c>
+      <c r="AF1" s="23" t="s">
+        <v>165</v>
       </c>
       <c r="AG1" s="3" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="AH1" s="3" t="s">
         <v>21</v>
@@ -3278,19 +3230,19 @@
         <v>29</v>
       </c>
       <c r="AJ1" s="3" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="AK1" s="3" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="AL1" s="3" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="AM1" s="3" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="AN1" s="3" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="AO1" s="3" t="s">
         <v>37</v>
@@ -3299,28 +3251,28 @@
         <v>38</v>
       </c>
       <c r="AQ1" s="3" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="AR1" s="3" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="AS1" s="3" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="AT1" s="2" t="s">
         <v>20</v>
       </c>
       <c r="AU1" s="2" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="AV1" s="2" t="s">
         <v>33</v>
       </c>
       <c r="AW1" s="3" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="AX1" s="3" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="AY1" s="2" t="s">
         <v>46</v>
@@ -3426,7 +3378,7 @@
       <c r="Z2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AA2" s="21" t="s">
+      <c r="AA2" s="23" t="s">
         <v>49</v>
       </c>
       <c r="AB2" s="3" t="s">
@@ -3441,7 +3393,7 @@
       <c r="AE2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AF2" s="21" t="s">
+      <c r="AF2" s="23" t="s">
         <v>49</v>
       </c>
       <c r="AG2" s="3" t="s">
@@ -3530,14 +3482,14 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="4" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="4" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="4" t="s">
@@ -3563,23 +3515,23 @@
       </c>
       <c r="X3" s="3"/>
       <c r="Y3" s="4" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="Z3" s="3"/>
-      <c r="AA3" s="22" t="n">
+      <c r="AA3" s="24" t="n">
         <v>100</v>
       </c>
-      <c r="AB3" s="23" t="n">
+      <c r="AB3" s="25" t="n">
         <v>1</v>
       </c>
       <c r="AC3" s="4" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="AD3" s="3"/>
       <c r="AE3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="AF3" s="22" t="n">
+      <c r="AF3" s="24" t="n">
         <v>1000</v>
       </c>
       <c r="AG3" s="3"/>
@@ -3627,31 +3579,31 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>179</v>
-      </c>
-      <c r="H4" s="24" t="s">
-        <v>180</v>
+        <v>185</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>187</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="K4" s="6" t="n">
         <v>100</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="N4" s="6" t="n">
         <v>1713</v>
@@ -3660,10 +3612,10 @@
         <v>100</v>
       </c>
       <c r="W4" s="6" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="Y4" s="6" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="AA4" s="6" t="n">
         <v>3500</v>
@@ -3687,36 +3639,36 @@
         <v>0</v>
       </c>
       <c r="AH4" s="6" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="AJ4" s="6" t="n">
         <v>1</v>
       </c>
       <c r="AT4" s="6" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="AY4" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="AZ4" s="24" t="s">
-        <v>188</v>
+        <v>194</v>
+      </c>
+      <c r="AZ4" s="26" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>191</v>
+        <v>178</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>198</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="K5" s="6" t="n">
         <v>100</v>
@@ -3731,10 +3683,10 @@
         <v>100</v>
       </c>
       <c r="W5" s="6" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="Y5" s="6" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="AA5" s="6" t="n">
         <v>1500</v>
@@ -3758,13 +3710,13 @@
         <v>0</v>
       </c>
       <c r="AH5" s="6" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="AJ5" s="6" t="n">
         <v>1</v>
       </c>
       <c r="AT5" s="6" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3772,22 +3724,22 @@
         <v>127</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="F6" s="24" t="s">
-        <v>198</v>
+        <v>178</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>205</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="K6" s="6" t="n">
         <v>100</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="N6" s="6" t="n">
         <v>549</v>
@@ -3796,10 +3748,10 @@
         <v>100</v>
       </c>
       <c r="W6" s="6" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="Y6" s="6" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="AA6" s="6" t="n">
         <v>1500</v>
@@ -3823,70 +3775,55 @@
         <v>0</v>
       </c>
       <c r="AH6" s="6" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AJ6" s="6" t="n">
         <v>1</v>
       </c>
       <c r="AV6" s="6" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="AY6" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="AZ6" s="24" t="s">
-        <v>205</v>
+        <v>211</v>
+      </c>
+      <c r="AZ6" s="26" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="C7" s="0"/>
-      <c r="D7" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="E7" s="0"/>
+      <c r="D7" s="21" t="s">
+        <v>178</v>
+      </c>
       <c r="F7" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="G7" s="0"/>
-      <c r="H7" s="0"/>
       <c r="I7" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="J7" s="0"/>
+        <v>214</v>
+      </c>
       <c r="K7" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="L7" s="0"/>
       <c r="M7" s="1" t="s">
         <v>123</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="O7" s="0"/>
-      <c r="P7" s="0"/>
-      <c r="Q7" s="0"/>
-      <c r="R7" s="0"/>
+        <v>215</v>
+      </c>
       <c r="S7" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="T7" s="0"/>
-      <c r="U7" s="0"/>
-      <c r="V7" s="0"/>
       <c r="W7" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="X7" s="0"/>
       <c r="Y7" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="Z7" s="0"/>
       <c r="AA7" s="1" t="n">
         <v>2686</v>
       </c>
@@ -3909,30 +3846,14 @@
         <v>0</v>
       </c>
       <c r="AH7" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="AI7" s="0"/>
+        <v>216</v>
+      </c>
       <c r="AJ7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AK7" s="0"/>
-      <c r="AL7" s="0"/>
-      <c r="AM7" s="0"/>
-      <c r="AN7" s="0"/>
-      <c r="AO7" s="0"/>
-      <c r="AP7" s="0"/>
-      <c r="AQ7" s="0"/>
-      <c r="AR7" s="0"/>
-      <c r="AS7" s="0"/>
       <c r="AT7" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="AU7" s="0"/>
-      <c r="AV7" s="0"/>
-      <c r="AW7" s="0"/>
-      <c r="AX7" s="0"/>
-      <c r="AY7" s="0"/>
-      <c r="AZ7" s="0"/>
+        <v>193</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3955,7 +3876,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H8" activeCellId="1" sqref="F7 H8"/>
+      <selection pane="bottomLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3987,215 +3908,215 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="C1" s="26" t="s">
+      <c r="A1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="C1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="26" t="s">
-        <v>211</v>
-      </c>
-      <c r="I1" s="26" t="s">
+      <c r="H1" s="27" t="s">
+        <v>218</v>
+      </c>
+      <c r="I1" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="J1" s="26" t="s">
-        <v>212</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>213</v>
-      </c>
-      <c r="L1" s="26" t="s">
-        <v>214</v>
-      </c>
-      <c r="M1" s="26" t="s">
-        <v>215</v>
-      </c>
-      <c r="N1" s="26" t="s">
-        <v>216</v>
-      </c>
-      <c r="O1" s="26" t="s">
+      <c r="J1" s="27" t="s">
+        <v>219</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="L1" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="M1" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="N1" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="O1" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="26" t="s">
-        <v>217</v>
-      </c>
-      <c r="Q1" s="26" t="s">
-        <v>218</v>
-      </c>
-      <c r="R1" s="26" t="s">
-        <v>219</v>
-      </c>
-      <c r="S1" s="26" t="s">
-        <v>220</v>
-      </c>
-      <c r="T1" s="26" t="s">
-        <v>221</v>
-      </c>
-      <c r="U1" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="V1" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="W1" s="26" t="s">
+      <c r="P1" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q1" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="R1" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="S1" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="T1" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="U1" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="V1" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="W1" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="X1" s="26" t="s">
+      <c r="X1" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="26" t="s">
+      <c r="A2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="26" t="s">
+      <c r="H2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="26" t="s">
+      <c r="J2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="L2" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="N2" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="O2" s="26" t="s">
+      <c r="L2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="P2" s="26" t="s">
+      <c r="P2" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="Q2" s="26" t="s">
+      <c r="Q2" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="R2" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="S2" s="26" t="s">
+      <c r="R2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="S2" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="T2" s="26" t="s">
+      <c r="T2" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="U2" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="V2" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="W2" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="X2" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
+      <c r="U2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="V2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="W2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="X2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y2" s="28"/>
+      <c r="Z2" s="28"/>
+      <c r="AA2" s="28"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="26" t="s">
-        <v>224</v>
-      </c>
-      <c r="F3" s="26" t="n">
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="F3" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="G3" s="26" t="n">
+      <c r="G3" s="27" t="n">
         <v>100</v>
       </c>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="26" t="s">
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="26" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" s="26" t="s">
-        <v>225</v>
-      </c>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="U3" s="27"/>
-      <c r="V3" s="27"/>
-      <c r="W3" s="27"/>
-      <c r="X3" s="27"/>
-      <c r="Y3" s="27"/>
-      <c r="Z3" s="27"/>
-      <c r="AA3" s="27"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="S3" s="28"/>
+      <c r="T3" s="28"/>
+      <c r="U3" s="28"/>
+      <c r="V3" s="28"/>
+      <c r="W3" s="28"/>
+      <c r="X3" s="28"/>
+      <c r="Y3" s="28"/>
+      <c r="Z3" s="28"/>
+      <c r="AA3" s="28"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>228</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>229</v>
+        <v>235</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>236</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="F4" s="6" t="n">
         <v>27</v>
@@ -4207,48 +4128,48 @@
         <v>0</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="L4" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="P4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="M4" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="P4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>225</v>
-      </c>
       <c r="S4" s="6" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="U4" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="V4" s="24" t="s">
-        <v>237</v>
+        <v>243</v>
+      </c>
+      <c r="V4" s="26" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>240</v>
+        <v>246</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>247</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="F5" s="6" t="n">
         <v>1</v>
@@ -4260,7 +4181,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="L5" s="6" t="s">
         <v>63</v>
@@ -4272,13 +4193,13 @@
         <v>0</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="V5" s="24" t="s">
-        <v>242</v>
+        <v>248</v>
+      </c>
+      <c r="V5" s="26" t="s">
+        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>